<commit_message>
Adding the section explaintion
</commit_message>
<xml_diff>
--- a/Main Files/Excel Files/تحكم بالاقسام.xlsx
+++ b/Main Files/Excel Files/تحكم بالاقسام.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Python\telegram bot for education\Your Work\student-helper-bot\Main Files\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{141B3B4B-0E53-4D9B-A618-8974757227C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{185CED9C-1AB4-4F81-B80B-01F69363B9AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4344" yWindow="1308" windowWidth="17892" windowHeight="9924" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
   <si>
     <t>section_path</t>
   </si>
@@ -84,6 +84,33 @@
   </si>
   <si>
     <t>design_for_you</t>
+  </si>
+  <si>
+    <t>تحديد المستوى</t>
+  </si>
+  <si>
+    <t>اختبار المستوى: اللفظي</t>
+  </si>
+  <si>
+    <t>اختبار المستوى: الكمي</t>
+  </si>
+  <si>
+    <t>الاختبارات</t>
+  </si>
+  <si>
+    <t>الاختبار: اللفظي</t>
+  </si>
+  <si>
+    <t>الاختبار: الكمي</t>
+  </si>
+  <si>
+    <t>نصائح واستراتيجيات</t>
+  </si>
+  <si>
+    <t>الإحصائيات</t>
+  </si>
+  <si>
+    <t>نصمملك</t>
   </si>
 </sst>
 </file>
@@ -498,7 +525,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -579,6 +606,9 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
       <c r="B5" t="s">
         <v>12</v>
       </c>
@@ -593,6 +623,9 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
       <c r="B6" t="s">
         <v>14</v>
       </c>
@@ -607,6 +640,9 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
       <c r="B7" t="s">
         <v>15</v>
       </c>
@@ -621,6 +657,9 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
       <c r="B8" t="s">
         <v>13</v>
       </c>
@@ -635,6 +674,9 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
       <c r="B9" t="s">
         <v>16</v>
       </c>
@@ -649,6 +691,9 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
       <c r="B10" t="s">
         <v>17</v>
       </c>
@@ -663,6 +708,9 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
       <c r="B11" t="s">
         <v>18</v>
       </c>
@@ -677,6 +725,9 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
       <c r="B12" t="s">
         <v>19</v>
       </c>
@@ -691,6 +742,9 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
       <c r="B13" t="s">
         <v>20</v>
       </c>

</xml_diff>